<commit_message>
Excel actualizado: Version Final
</commit_message>
<xml_diff>
--- a/docs/Tests Cases.xlsx
+++ b/docs/Tests Cases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\talib\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B5018E16-789C-45B5-BE1A-79B2268A43A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{12AA98A5-1EA1-431A-BBE8-2E4E4F97723A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20910" yWindow="1965" windowWidth="20460" windowHeight="13695" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GE3 2021 F1" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="127">
   <si>
     <t>#</t>
   </si>
@@ -70,9 +70,6 @@
   </si>
   <si>
     <t>ENTRADA</t>
-  </si>
-  <si>
-    <t>EC</t>
   </si>
   <si>
     <t>VALID</t>
@@ -392,6 +389,29 @@
   <si>
     <t>Comprueba el caso en el que el hash que devuelve 
 la funcion requestvaccination es distinto</t>
+  </si>
+  <si>
+    <t>CN</t>
+  </si>
+  <si>
+    <t>str(UUID4) / otros</t>
+  </si>
+  <si>
+    <t>int(6&lt;=x&lt;=120) /otros</t>
+  </si>
+  <si>
+    <t>len(str(*más de una palabra*))&lt;30 
+/ otros</t>
+  </si>
+  <si>
+    <t>Todos los datos correctos / 
+Algún dato incorrecto</t>
+  </si>
+  <si>
+    <t>len(str("1-9"))==9 / otros</t>
+  </si>
+  <si>
+    <t>str("Regular") or str("Family") / otros</t>
   </si>
 </sst>
 </file>
@@ -429,7 +449,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -445,6 +465,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -489,7 +515,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -544,6 +570,13 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1239,7 +1272,7 @@
   <dimension ref="A1:O1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O24" sqref="O24"/>
+      <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.109375" defaultRowHeight="15" customHeight="1"/>
@@ -1247,7 +1280,7 @@
     <col min="1" max="2" width="10.5546875" customWidth="1"/>
     <col min="3" max="3" width="9.5546875" customWidth="1"/>
     <col min="4" max="4" width="17.109375" customWidth="1"/>
-    <col min="5" max="5" width="11.33203125" customWidth="1"/>
+    <col min="5" max="5" width="29.6640625" customWidth="1"/>
     <col min="6" max="6" width="25.33203125" customWidth="1"/>
     <col min="7" max="7" width="24.6640625" customWidth="1"/>
     <col min="8" max="8" width="70.33203125" style="4" customWidth="1"/>
@@ -1274,7 +1307,7 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="21" t="s">
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
@@ -1315,32 +1348,32 @@
       <c r="B2" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="9" t="s">
-        <v>16</v>
+      <c r="C2" s="20" t="s">
+        <v>120</v>
       </c>
       <c r="D2" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="9" t="s">
+      <c r="E2" s="20" t="s">
+        <v>121</v>
+      </c>
+      <c r="F2" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="F2" s="9" t="s">
+      <c r="G2" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="G2" s="9" t="s">
+      <c r="H2" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="H2" s="10" t="s">
+      <c r="I2" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="I2" s="9" t="s">
+      <c r="J2" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="J2" s="9" t="s">
+      <c r="K2" s="9" t="s">
         <v>22</v>
-      </c>
-      <c r="K2" s="9" t="s">
-        <v>23</v>
       </c>
       <c r="L2" s="9">
         <v>123456789</v>
@@ -1349,7 +1382,7 @@
         <v>20</v>
       </c>
       <c r="N2" s="9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="O2" s="11"/>
     </row>
@@ -1358,34 +1391,34 @@
         <v>2</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>16</v>
+        <v>120</v>
       </c>
       <c r="D3" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="9" t="s">
-        <v>17</v>
+      <c r="E3" s="20" t="s">
+        <v>121</v>
       </c>
       <c r="F3" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G3" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="G3" s="9" t="s">
+      <c r="H3" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="H3" s="12" t="s">
+      <c r="I3" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="I3" s="9" t="s">
-        <v>29</v>
-      </c>
       <c r="J3" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="K3" s="9" t="s">
         <v>22</v>
-      </c>
-      <c r="K3" s="9" t="s">
-        <v>23</v>
       </c>
       <c r="L3" s="9">
         <v>123456789</v>
@@ -1394,7 +1427,7 @@
         <v>20</v>
       </c>
       <c r="N3" s="9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="O3" s="11"/>
     </row>
@@ -1405,32 +1438,32 @@
       <c r="B4" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="9" t="s">
-        <v>16</v>
+      <c r="C4" s="20" t="s">
+        <v>120</v>
       </c>
       <c r="D4" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="9" t="s">
-        <v>17</v>
+      <c r="E4" s="20" t="s">
+        <v>122</v>
       </c>
       <c r="F4" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="G4" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="G4" s="9" t="s">
+      <c r="H4" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="H4" s="12" t="s">
-        <v>32</v>
-      </c>
       <c r="I4" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J4" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="K4" s="9" t="s">
         <v>22</v>
-      </c>
-      <c r="K4" s="9" t="s">
-        <v>23</v>
       </c>
       <c r="L4" s="9">
         <v>123456789</v>
@@ -1439,7 +1472,7 @@
         <v>4</v>
       </c>
       <c r="N4" s="9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="O4" s="11"/>
     </row>
@@ -1451,31 +1484,31 @@
         <v>15</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>16</v>
+        <v>120</v>
       </c>
       <c r="D5" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="9" t="s">
-        <v>17</v>
+      <c r="E5" s="20" t="s">
+        <v>122</v>
       </c>
       <c r="F5" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="G5" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="G5" s="9" t="s">
+      <c r="H5" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="H5" s="12" t="s">
-        <v>35</v>
-      </c>
       <c r="I5" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J5" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="K5" s="9" t="s">
         <v>22</v>
-      </c>
-      <c r="K5" s="9" t="s">
-        <v>23</v>
       </c>
       <c r="L5" s="9">
         <v>123456789</v>
@@ -1484,7 +1517,7 @@
         <v>150</v>
       </c>
       <c r="N5" s="9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="O5" s="11"/>
     </row>
@@ -1495,45 +1528,45 @@
       <c r="B6" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="9" t="s">
-        <v>16</v>
+      <c r="C6" s="20" t="s">
+        <v>120</v>
       </c>
       <c r="D6" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="E6" s="9" t="s">
-        <v>17</v>
+      <c r="E6" s="20" t="s">
+        <v>122</v>
       </c>
       <c r="F6" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="G6" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="G6" s="9" t="s">
+      <c r="H6" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="H6" s="12" t="s">
-        <v>38</v>
-      </c>
       <c r="I6" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J6" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="K6" s="9" t="s">
         <v>22</v>
-      </c>
-      <c r="K6" s="9" t="s">
-        <v>23</v>
       </c>
       <c r="L6" s="9">
         <v>123456789</v>
       </c>
       <c r="M6" s="9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="N6" s="9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="O6" s="11"/>
     </row>
-    <row r="7" spans="1:15" ht="19.7" customHeight="1">
+    <row r="7" spans="1:15" ht="41.25" customHeight="1">
       <c r="A7" s="9">
         <v>6</v>
       </c>
@@ -1541,31 +1574,31 @@
         <v>15</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>16</v>
+        <v>120</v>
       </c>
       <c r="D7" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="E7" s="9" t="s">
-        <v>17</v>
+      <c r="E7" s="10" t="s">
+        <v>123</v>
       </c>
       <c r="F7" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="G7" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="G7" s="9" t="s">
+      <c r="H7" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="H7" s="12" t="s">
+      <c r="I7" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="J7" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="K7" s="9" t="s">
         <v>42</v>
-      </c>
-      <c r="I7" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="J7" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="K7" s="9" t="s">
-        <v>43</v>
       </c>
       <c r="L7" s="9">
         <v>123456789</v>
@@ -1574,43 +1607,43 @@
         <v>20</v>
       </c>
       <c r="N7" s="9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="O7" s="11"/>
     </row>
-    <row r="8" spans="1:15" ht="19.7" customHeight="1">
+    <row r="8" spans="1:15" ht="41.25" customHeight="1">
       <c r="A8" s="9">
         <v>7</v>
       </c>
       <c r="B8" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="9" t="s">
-        <v>16</v>
+      <c r="C8" s="20" t="s">
+        <v>120</v>
       </c>
       <c r="D8" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="E8" s="9" t="s">
-        <v>17</v>
+      <c r="E8" s="10" t="s">
+        <v>123</v>
       </c>
       <c r="F8" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="G8" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="G8" s="9" t="s">
+      <c r="H8" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="H8" s="12" t="s">
+      <c r="I8" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="J8" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="K8" s="9" t="s">
         <v>46</v>
-      </c>
-      <c r="I8" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="J8" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="K8" s="9" t="s">
-        <v>47</v>
       </c>
       <c r="L8" s="9">
         <v>123456789</v>
@@ -1619,11 +1652,11 @@
         <v>20</v>
       </c>
       <c r="N8" s="9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="O8" s="11"/>
     </row>
-    <row r="9" spans="1:15" ht="19.7" customHeight="1">
+    <row r="9" spans="1:15" ht="37.5" customHeight="1">
       <c r="A9" s="9">
         <v>8</v>
       </c>
@@ -1631,31 +1664,31 @@
         <v>15</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>16</v>
+        <v>120</v>
       </c>
       <c r="D9" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="E9" s="9" t="s">
-        <v>17</v>
+      <c r="E9" s="10" t="s">
+        <v>123</v>
       </c>
       <c r="F9" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="G9" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="G9" s="9" t="s">
+      <c r="H9" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="H9" s="12" t="s">
+      <c r="I9" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="J9" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="K9" s="9" t="s">
         <v>50</v>
-      </c>
-      <c r="I9" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="J9" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="K9" s="9" t="s">
-        <v>51</v>
       </c>
       <c r="L9" s="9">
         <v>123456789</v>
@@ -1664,7 +1697,7 @@
         <v>20</v>
       </c>
       <c r="N9" s="9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="O9" s="11"/>
     </row>
@@ -1675,32 +1708,32 @@
       <c r="B10" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="C10" s="9" t="s">
-        <v>16</v>
+      <c r="C10" s="20" t="s">
+        <v>120</v>
       </c>
       <c r="D10" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="E10" s="9" t="s">
-        <v>17</v>
+      <c r="E10" s="20" t="s">
+        <v>121</v>
       </c>
       <c r="F10" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="G10" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="H10" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="G10" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="H10" s="10" t="s">
+      <c r="I10" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="I10" s="9" t="s">
-        <v>54</v>
-      </c>
       <c r="J10" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="K10" s="9" t="s">
         <v>22</v>
-      </c>
-      <c r="K10" s="9" t="s">
-        <v>23</v>
       </c>
       <c r="L10" s="9">
         <v>123456789</v>
@@ -1709,43 +1742,43 @@
         <v>20</v>
       </c>
       <c r="N10" s="9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="O10" s="11"/>
     </row>
-    <row r="11" spans="1:15" ht="19.7" customHeight="1">
+    <row r="11" spans="1:15" ht="40.5" customHeight="1">
       <c r="A11" s="9">
         <v>10</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>16</v>
+        <v>120</v>
       </c>
       <c r="D11" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="E11" s="10" t="s">
+        <v>124</v>
+      </c>
+      <c r="F11" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="E11" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="F11" s="9" t="s">
+      <c r="G11" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="G11" s="9" t="s">
+      <c r="H11" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="H11" s="12" t="s">
-        <v>58</v>
-      </c>
       <c r="I11" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J11" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="K11" s="9" t="s">
         <v>22</v>
-      </c>
-      <c r="K11" s="9" t="s">
-        <v>23</v>
       </c>
       <c r="L11" s="9">
         <v>123456789</v>
@@ -1754,10 +1787,10 @@
         <v>20</v>
       </c>
       <c r="N11" s="9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="O11" s="20" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="12" spans="1:15" ht="19.7" customHeight="1">
@@ -1767,32 +1800,32 @@
       <c r="B12" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="C12" s="9" t="s">
-        <v>16</v>
+      <c r="C12" s="20" t="s">
+        <v>120</v>
       </c>
       <c r="D12" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="E12" s="9" t="s">
-        <v>17</v>
+      <c r="E12" s="20" t="s">
+        <v>125</v>
       </c>
       <c r="F12" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="G12" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="G12" s="9" t="s">
+      <c r="H12" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="H12" s="12" t="s">
-        <v>62</v>
-      </c>
       <c r="I12" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J12" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="K12" s="9" t="s">
         <v>22</v>
-      </c>
-      <c r="K12" s="9" t="s">
-        <v>23</v>
       </c>
       <c r="L12" s="9">
         <v>624</v>
@@ -1801,7 +1834,7 @@
         <v>20</v>
       </c>
       <c r="N12" s="9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="O12" s="11"/>
     </row>
@@ -1813,40 +1846,40 @@
         <v>15</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>16</v>
+        <v>120</v>
       </c>
       <c r="D13" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="E13" s="9" t="s">
-        <v>17</v>
+      <c r="E13" s="20" t="s">
+        <v>125</v>
       </c>
       <c r="F13" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="G13" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="G13" s="9" t="s">
+      <c r="H13" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="H13" s="12" t="s">
+      <c r="I13" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="J13" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="K13" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="L13" s="9" t="s">
         <v>65</v>
-      </c>
-      <c r="I13" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="J13" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="K13" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="L13" s="9" t="s">
-        <v>66</v>
       </c>
       <c r="M13" s="9">
         <v>20</v>
       </c>
       <c r="N13" s="9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="O13" s="11"/>
     </row>
@@ -1857,41 +1890,41 @@
       <c r="B14" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="C14" s="9" t="s">
-        <v>16</v>
+      <c r="C14" s="20" t="s">
+        <v>120</v>
       </c>
       <c r="D14" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="E14" s="9" t="s">
-        <v>17</v>
+      <c r="E14" s="20" t="s">
+        <v>125</v>
       </c>
       <c r="F14" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="G14" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="G14" s="9" t="s">
+      <c r="H14" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="H14" s="12" t="s">
+      <c r="I14" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="J14" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="K14" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="L14" s="9" t="s">
         <v>69</v>
-      </c>
-      <c r="I14" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="J14" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="K14" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="L14" s="9" t="s">
-        <v>70</v>
       </c>
       <c r="M14" s="9">
         <v>20</v>
       </c>
       <c r="N14" s="9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="O14" s="11"/>
     </row>
@@ -1903,31 +1936,31 @@
         <v>15</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>16</v>
+        <v>120</v>
       </c>
       <c r="D15" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="E15" s="9" t="s">
-        <v>17</v>
+      <c r="E15" s="20" t="s">
+        <v>126</v>
       </c>
       <c r="F15" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="G15" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="G15" s="9" t="s">
+      <c r="H15" s="12" t="s">
         <v>72</v>
       </c>
-      <c r="H15" s="12" t="s">
+      <c r="I15" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="J15" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="I15" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="J15" s="9" t="s">
-        <v>74</v>
-      </c>
       <c r="K15" s="9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="L15" s="9">
         <v>123456789</v>
@@ -1936,7 +1969,7 @@
         <v>20</v>
       </c>
       <c r="N15" s="9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="O15" s="11"/>
     </row>
@@ -1947,32 +1980,32 @@
       <c r="B16" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="C16" s="9" t="s">
-        <v>16</v>
+      <c r="C16" s="20" t="s">
+        <v>120</v>
       </c>
       <c r="D16" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="E16" s="9" t="s">
-        <v>17</v>
+      <c r="E16" s="20" t="s">
+        <v>126</v>
       </c>
       <c r="F16" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="G16" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="G16" s="9" t="s">
+      <c r="H16" s="12" t="s">
         <v>76</v>
       </c>
-      <c r="H16" s="12" t="s">
-        <v>77</v>
-      </c>
       <c r="I16" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J16" s="15">
         <v>12</v>
       </c>
       <c r="K16" s="9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="L16" s="9">
         <v>123456789</v>
@@ -1981,43 +2014,43 @@
         <v>20</v>
       </c>
       <c r="N16" s="9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="O16" s="11"/>
     </row>
-    <row r="17" spans="1:15" ht="19.7" customHeight="1">
+    <row r="17" spans="1:15" ht="42.75" customHeight="1">
       <c r="A17" s="9">
         <v>16</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>16</v>
+        <v>120</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="E17" s="9" t="s">
-        <v>17</v>
+        <v>54</v>
+      </c>
+      <c r="E17" s="10" t="s">
+        <v>124</v>
       </c>
       <c r="F17" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="G17" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="H17" s="12" t="s">
         <v>78</v>
       </c>
-      <c r="G17" s="9" t="s">
-        <v>57</v>
-      </c>
-      <c r="H17" s="12" t="s">
-        <v>79</v>
-      </c>
       <c r="I17" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J17" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="K17" s="9" t="s">
         <v>22</v>
-      </c>
-      <c r="K17" s="9" t="s">
-        <v>23</v>
       </c>
       <c r="L17" s="9">
         <v>123456789</v>
@@ -2026,45 +2059,45 @@
         <v>20</v>
       </c>
       <c r="N17" s="9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="O17" s="13" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="18" spans="1:15" ht="19.7" customHeight="1">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" ht="41.25" customHeight="1">
       <c r="A18" s="9">
         <v>17</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="C18" s="9" t="s">
-        <v>16</v>
+        <v>24</v>
+      </c>
+      <c r="C18" s="20" t="s">
+        <v>120</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="E18" s="9" t="s">
-        <v>17</v>
+        <v>54</v>
+      </c>
+      <c r="E18" s="10" t="s">
+        <v>124</v>
       </c>
       <c r="F18" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="G18" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="G18" s="9" t="s">
+      <c r="H18" s="12" t="s">
         <v>81</v>
       </c>
-      <c r="H18" s="12" t="s">
-        <v>82</v>
-      </c>
       <c r="I18" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J18" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="K18" s="9" t="s">
         <v>22</v>
-      </c>
-      <c r="K18" s="9" t="s">
-        <v>23</v>
       </c>
       <c r="L18" s="9">
         <v>123456789</v>
@@ -2073,43 +2106,43 @@
         <v>20</v>
       </c>
       <c r="N18" s="9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="O18" s="11"/>
     </row>
-    <row r="19" spans="1:15" ht="19.7" customHeight="1">
+    <row r="19" spans="1:15" ht="40.5" customHeight="1">
       <c r="A19" s="9">
         <v>18</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>16</v>
+        <v>120</v>
       </c>
       <c r="D19" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="E19" s="9" t="s">
-        <v>17</v>
+        <v>54</v>
+      </c>
+      <c r="E19" s="10" t="s">
+        <v>124</v>
       </c>
       <c r="F19" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="G19" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="G19" s="9" t="s">
+      <c r="H19" s="12" t="s">
         <v>84</v>
       </c>
-      <c r="H19" s="12" t="s">
-        <v>85</v>
-      </c>
       <c r="I19" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J19" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="K19" s="9" t="s">
         <v>22</v>
-      </c>
-      <c r="K19" s="9" t="s">
-        <v>23</v>
       </c>
       <c r="L19" s="9">
         <v>123456789</v>
@@ -2118,43 +2151,43 @@
         <v>20</v>
       </c>
       <c r="N19" s="9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="O19" s="11"/>
     </row>
-    <row r="20" spans="1:15" ht="19.7" customHeight="1">
+    <row r="20" spans="1:15" ht="41.25" customHeight="1">
       <c r="A20" s="9">
         <v>19</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="C20" s="9" t="s">
-        <v>16</v>
+        <v>24</v>
+      </c>
+      <c r="C20" s="20" t="s">
+        <v>120</v>
       </c>
       <c r="D20" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="E20" s="9" t="s">
-        <v>17</v>
+        <v>54</v>
+      </c>
+      <c r="E20" s="10" t="s">
+        <v>124</v>
       </c>
       <c r="F20" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="G20" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="G20" s="9" t="s">
+      <c r="H20" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="H20" s="12" t="s">
-        <v>88</v>
-      </c>
       <c r="I20" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J20" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="K20" s="9" t="s">
         <v>22</v>
-      </c>
-      <c r="K20" s="9" t="s">
-        <v>23</v>
       </c>
       <c r="L20" s="9">
         <v>123456789</v>
@@ -2163,7 +2196,7 @@
         <v>20</v>
       </c>
       <c r="N20" s="9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="O20" s="11"/>
     </row>
@@ -2172,34 +2205,34 @@
         <v>20</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>16</v>
+        <v>120</v>
       </c>
       <c r="D21" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="E21" s="9" t="s">
-        <v>17</v>
+        <v>54</v>
+      </c>
+      <c r="E21" s="10" t="s">
+        <v>124</v>
       </c>
       <c r="F21" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="G21" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="G21" s="9" t="s">
-        <v>90</v>
-      </c>
       <c r="H21" s="10" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="I21" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J21" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="K21" s="9" t="s">
         <v>22</v>
-      </c>
-      <c r="K21" s="9" t="s">
-        <v>23</v>
       </c>
       <c r="L21" s="9">
         <v>123456789</v>
@@ -2208,7 +2241,7 @@
         <v>32</v>
       </c>
       <c r="N21" s="9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="O21" s="11"/>
     </row>
@@ -2219,32 +2252,32 @@
       <c r="B22" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="C22" s="9" t="s">
-        <v>16</v>
+      <c r="C22" s="20" t="s">
+        <v>120</v>
       </c>
       <c r="D22" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="E22" s="9" t="s">
-        <v>17</v>
+      <c r="E22" s="20" t="s">
+        <v>122</v>
       </c>
       <c r="F22" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="G22" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="H22" s="12" t="s">
         <v>91</v>
       </c>
-      <c r="G22" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="H22" s="12" t="s">
-        <v>92</v>
-      </c>
       <c r="I22" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J22" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="K22" s="9" t="s">
         <v>22</v>
-      </c>
-      <c r="K22" s="9" t="s">
-        <v>23</v>
       </c>
       <c r="L22" s="9">
         <v>123456789</v>
@@ -2253,11 +2286,11 @@
         <v>44615</v>
       </c>
       <c r="N22" s="9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="O22" s="11"/>
     </row>
-    <row r="23" spans="1:15" ht="19.7" customHeight="1">
+    <row r="23" spans="1:15" ht="37.5" customHeight="1">
       <c r="A23" s="9">
         <v>22</v>
       </c>
@@ -2265,28 +2298,28 @@
         <v>15</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>16</v>
+        <v>120</v>
       </c>
       <c r="D23" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="E23" s="9" t="s">
-        <v>17</v>
+      <c r="E23" s="10" t="s">
+        <v>123</v>
       </c>
       <c r="F23" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="G23" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="G23" s="9" t="s">
+      <c r="H23" s="12" t="s">
         <v>94</v>
       </c>
-      <c r="H23" s="12" t="s">
-        <v>95</v>
-      </c>
       <c r="I23" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J23" s="9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K23" s="9">
         <v>1234567</v>
@@ -2298,7 +2331,7 @@
         <v>20</v>
       </c>
       <c r="N23" s="9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="O23" s="11"/>
     </row>
@@ -2309,32 +2342,32 @@
       <c r="B24" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="C24" s="17" t="s">
-        <v>16</v>
+      <c r="C24" s="20" t="s">
+        <v>120</v>
       </c>
       <c r="D24" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="E24" s="17" t="s">
-        <v>17</v>
+      <c r="E24" s="20" t="s">
+        <v>121</v>
       </c>
       <c r="F24" s="17" t="s">
+        <v>95</v>
+      </c>
+      <c r="G24" s="17" t="s">
         <v>96</v>
       </c>
-      <c r="G24" s="17" t="s">
+      <c r="H24" s="18" t="s">
         <v>97</v>
-      </c>
-      <c r="H24" s="18" t="s">
-        <v>98</v>
       </c>
       <c r="I24" s="17">
         <v>382843292</v>
       </c>
       <c r="J24" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="K24" s="17" t="s">
         <v>22</v>
-      </c>
-      <c r="K24" s="17" t="s">
-        <v>23</v>
       </c>
       <c r="L24" s="17">
         <v>123456789</v>
@@ -2343,14 +2376,14 @@
         <v>20</v>
       </c>
       <c r="N24" s="17" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="O24" s="19"/>
     </row>
     <row r="25" spans="1:15" ht="15.75" customHeight="1">
       <c r="A25" s="5"/>
       <c r="B25" s="5"/>
-      <c r="C25" s="5"/>
+      <c r="C25" s="22"/>
       <c r="D25" s="5"/>
       <c r="E25" s="5"/>
       <c r="F25" s="5"/>
@@ -2388,8 +2421,8 @@
       <c r="D27" s="5"/>
       <c r="E27" s="5"/>
       <c r="F27" s="5"/>
-      <c r="G27" s="5" t="s">
-        <v>99</v>
+      <c r="G27" s="23" t="s">
+        <v>98</v>
       </c>
       <c r="H27" s="6"/>
       <c r="I27" s="5"/>
@@ -2407,8 +2440,8 @@
       <c r="D28" s="5"/>
       <c r="E28" s="5"/>
       <c r="F28" s="5"/>
-      <c r="G28" s="5" t="s">
-        <v>100</v>
+      <c r="G28" s="23" t="s">
+        <v>99</v>
       </c>
       <c r="H28" s="6"/>
       <c r="I28" s="5"/>
@@ -2426,8 +2459,8 @@
       <c r="D29" s="5"/>
       <c r="E29" s="5"/>
       <c r="F29" s="5"/>
-      <c r="G29" s="5" t="s">
-        <v>101</v>
+      <c r="G29" s="23" t="s">
+        <v>100</v>
       </c>
       <c r="H29" s="6"/>
       <c r="I29" s="5"/>
@@ -3666,13 +3699,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>103</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>104</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>5</v>
@@ -3681,13 +3714,13 @@
         <v>7</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>106</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>107</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>14</v>
@@ -3701,25 +3734,25 @@
         <v>5</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>112</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>113</v>
       </c>
       <c r="J2" s="1"/>
     </row>
@@ -5211,7 +5244,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>5</v>
@@ -5220,10 +5253,10 @@
         <v>7</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>14</v>
@@ -5234,17 +5267,17 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>118</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>119</v>
       </c>
       <c r="G2" s="1"/>
     </row>

</xml_diff>